<commit_message>
Third step is a really good use of the Groupby function.
</commit_message>
<xml_diff>
--- a/CH-135 Identify the Pattern.xlsx
+++ b/CH-135 Identify the Pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339E2FA7-4222-4152-AF28-ADB99AE15E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C932A7-6AEC-40A4-BFFF-809ACD8B7AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="46">
   <si>
     <t>Question</t>
   </si>
@@ -198,6 +198,12 @@
   <si>
     <t>Work on understanding the filter array.</t>
   </si>
+  <si>
+    <t>I removed the total.</t>
+  </si>
+  <si>
+    <t>The scan is a great way to form the concatenated array.</t>
+  </si>
 </sst>
 </file>
 
@@ -206,7 +212,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +261,13 @@
       <color theme="10"/>
       <name val="Gill Sans"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -417,13 +430,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -467,6 +481,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,11 +493,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Intro_Hd" xfId="2" xr:uid="{3AFDA2A8-9D99-45A4-AE8C-38EB43CB03D4}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2579,6 +2595,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -2611,16 +2630,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
@@ -9105,19 +9124,19 @@
   <sheetData>
     <row r="1" spans="1:28" ht="22.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="23"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="19" t="s">
         <v>41</v>
       </c>
       <c r="M1" s="1"/>
@@ -17709,16 +17728,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
@@ -24222,16 +24241,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
@@ -30725,8 +30744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0764AA4C-3652-437B-BFCE-9D98C453175D}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -30744,16 +30763,16 @@
   <sheetData>
     <row r="1" spans="1:26" ht="22.5" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1" t="s">
@@ -31100,14 +31119,14 @@
       </c>
       <c r="E11" s="10"/>
       <c r="G11" t="str" cm="1">
-        <f t="array" aca="1" ref="G11:H14" ca="1">_xlfn.LET(
+        <f t="array" aca="1" ref="G11:H13" ca="1">_xlfn.LET(
     _xlpm.p, C3:C32,
     _xlfn.GROUPBY(
         _xlpm.p,
         _xlpm.p,
         _xleta.COUNTA,
         ,
-        ,
+        0,
         ,
         _xlfn.SCAN(, D3:D32, _xlfn.LAMBDA(_xlpm.x,_xlpm.y, _xlfn.CONCAT(OFFSET(_xlpm.y, , , -3)))) =
             "+-+"
@@ -31118,6 +31137,9 @@
       <c r="H11">
         <f ca="1"/>
         <v>1</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -31156,6 +31178,9 @@
         <f ca="1"/>
         <v>2</v>
       </c>
+      <c r="J12" s="25" t="s">
+        <v>45</v>
+      </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -31204,14 +31229,6 @@
         <v>8</v>
       </c>
       <c r="E14" s="13"/>
-      <c r="G14" t="str">
-        <f ca="1"/>
-        <v>Total</v>
-      </c>
-      <c r="H14">
-        <f ca="1"/>
-        <v>7</v>
-      </c>
     </row>
     <row r="15" spans="1:26" ht="17.25" customHeight="1">
       <c r="A15" s="14"/>

</xml_diff>

<commit_message>
Alt2 is the most clever regex. I would never have come up with this approach.
</commit_message>
<xml_diff>
--- a/CH-135 Identify the Pattern.xlsx
+++ b/CH-135 Identify the Pattern.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C932A7-6AEC-40A4-BFFF-809ACD8B7AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28BE575-2D03-4DCE-BC83-169229CAA1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="47">
   <si>
     <t>Question</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>The scan is a great way to form the concatenated array.</t>
+  </si>
+  <si>
+    <t>This is a very interesting regex.</t>
   </si>
 </sst>
 </file>
@@ -24222,8 +24225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952D5B38-5A13-4C24-A44A-CBF253B4ECC1}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -24504,7 +24507,9 @@
       </c>
       <c r="E8" s="10"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -24562,7 +24567,10 @@
       </c>
       <c r="E10" s="10"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="L10" s="2" t="str">
+        <f>_xlfn.CONCAT(C3:D32)</f>
+        <v>A+A+A-A-A+A-A-A+A-A+B-B+B-B+B-B-B-B+B+B-C+C-C+C-C+C-C+C-C-C+</v>
+      </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
@@ -24663,6 +24671,26 @@
       <c r="H13">
         <v>1</v>
       </c>
+      <c r="L13" t="str" cm="1">
+        <f t="array" ref="L13:P13" xml:space="preserve">        _xlfn.REGEXEXTRACT(
+            _xlfn.CONCAT(C3:D32),
+            "(.)(?=\+\1\-\1\+)",
+            1
+        )</f>
+        <v>A</v>
+      </c>
+      <c r="M13" t="str">
+        <v>B</v>
+      </c>
+      <c r="N13" t="str">
+        <v>C</v>
+      </c>
+      <c r="O13" t="str">
+        <v>C</v>
+      </c>
+      <c r="P13" t="str">
+        <v>C</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="17.25" customHeight="1">
       <c r="B14" s="8" t="s">
@@ -24701,6 +24729,17 @@
       <c r="H15">
         <v>3</v>
       </c>
+      <c r="L15" t="str" cm="1">
+        <f t="array" ref="L15:L19">_xlfn.TOCOL(_xlfn.ANCHORARRAY(L13))</f>
+        <v>A</v>
+      </c>
+      <c r="M15" t="str" cm="1">
+        <f t="array" ref="M15:N17">_xlfn.GROUPBY(_xlfn.ANCHORARRAY(L15),_xlfn.ANCHORARRAY( L15), _xleta.ROWS, , 0)</f>
+        <v>A</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="17.25" customHeight="1">
       <c r="A16" s="14"/>
@@ -24715,8 +24754,17 @@
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" ht="17.25" customHeight="1">
+      <c r="L16" t="str">
+        <v>B</v>
+      </c>
+      <c r="M16" t="str">
+        <v>B</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17.25" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="8" t="s">
         <v>25</v>
@@ -24729,8 +24777,17 @@
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" ht="17.25" customHeight="1">
+      <c r="L17" t="str">
+        <v>C</v>
+      </c>
+      <c r="M17" t="str">
+        <v>C</v>
+      </c>
+      <c r="N17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17.25" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="8" t="s">
         <v>26</v>
@@ -24743,8 +24800,11 @@
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" ht="17.25" customHeight="1">
+      <c r="L18" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="17.25" customHeight="1">
       <c r="A19" s="14"/>
       <c r="B19" s="8" t="s">
         <v>27</v>
@@ -24757,8 +24817,11 @@
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" ht="17.25" customHeight="1">
+      <c r="L19" t="str">
+        <v>C</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="17.25" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="8" t="s">
         <v>28</v>
@@ -24772,7 +24835,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
     </row>
-    <row r="21" spans="1:6" ht="17.25" customHeight="1">
+    <row r="21" spans="1:14" ht="17.25" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="8" t="s">
         <v>29</v>
@@ -24786,7 +24849,7 @@
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
     </row>
-    <row r="22" spans="1:6" ht="17.25" customHeight="1">
+    <row r="22" spans="1:14" ht="17.25" customHeight="1">
       <c r="A22" s="14"/>
       <c r="B22" s="8" t="s">
         <v>30</v>
@@ -24800,7 +24863,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
     </row>
-    <row r="23" spans="1:6" ht="17.25" customHeight="1">
+    <row r="23" spans="1:14" ht="17.25" customHeight="1">
       <c r="B23" s="8" t="s">
         <v>31</v>
       </c>
@@ -24813,7 +24876,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
     </row>
-    <row r="24" spans="1:6" ht="17.25" customHeight="1">
+    <row r="24" spans="1:14" ht="17.25" customHeight="1">
       <c r="B24" s="8" t="s">
         <v>32</v>
       </c>
@@ -24825,7 +24888,7 @@
       </c>
       <c r="F24" s="15"/>
     </row>
-    <row r="25" spans="1:6" ht="17.25" customHeight="1">
+    <row r="25" spans="1:14" ht="17.25" customHeight="1">
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
@@ -24837,7 +24900,7 @@
       </c>
       <c r="F25" s="15"/>
     </row>
-    <row r="26" spans="1:6" ht="17.25" customHeight="1">
+    <row r="26" spans="1:14" ht="17.25" customHeight="1">
       <c r="B26" s="8" t="s">
         <v>34</v>
       </c>
@@ -24849,7 +24912,7 @@
       </c>
       <c r="F26" s="15"/>
     </row>
-    <row r="27" spans="1:6" ht="17.25" customHeight="1">
+    <row r="27" spans="1:14" ht="17.25" customHeight="1">
       <c r="B27" s="8" t="s">
         <v>35</v>
       </c>
@@ -24861,7 +24924,7 @@
       </c>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:6" ht="17.25" customHeight="1">
+    <row r="28" spans="1:14" ht="17.25" customHeight="1">
       <c r="B28" s="8" t="s">
         <v>36</v>
       </c>
@@ -24873,7 +24936,7 @@
       </c>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" ht="17.25" customHeight="1">
+    <row r="29" spans="1:14" ht="17.25" customHeight="1">
       <c r="B29" s="8" t="s">
         <v>37</v>
       </c>
@@ -24885,7 +24948,7 @@
       </c>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" spans="1:6" ht="17.25" customHeight="1">
+    <row r="30" spans="1:14" ht="17.25" customHeight="1">
       <c r="B30" s="8" t="s">
         <v>38</v>
       </c>
@@ -24897,7 +24960,7 @@
       </c>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:6" ht="17.25" customHeight="1">
+    <row r="31" spans="1:14" ht="17.25" customHeight="1">
       <c r="B31" s="8" t="s">
         <v>39</v>
       </c>
@@ -24909,7 +24972,7 @@
       </c>
       <c r="F31" s="15"/>
     </row>
-    <row r="32" spans="1:6" ht="17.25" customHeight="1">
+    <row r="32" spans="1:14" ht="17.25" customHeight="1">
       <c r="B32" s="8" t="s">
         <v>40</v>
       </c>
@@ -30744,8 +30807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0764AA4C-3652-437B-BFCE-9D98C453175D}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>